<commit_message>
Support to skip special characters
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_01.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_01.xlsx
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>EXACT ("[petName]","Ethan")</t>
+  </si>
+  <si>
+    <t>petId|petName;1000|Test1;2000|Test2</t>
+  </si>
+  <si>
+    <t>EXACT ("[petName]","Test2")</t>
+  </si>
+  <si>
+    <t>petId|petName;i~1000|Test1;i~2000|Test2</t>
   </si>
 </sst>
 </file>
@@ -493,7 +502,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" sqref="L3"/>
+      <selection pane="topLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -575,10 +584,10 @@
         <v>201</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>